<commit_message>
Renaming cases file and cohorts
</commit_message>
<xml_diff>
--- a/residential measures/SWWH013-04 Tankless Water Heater/SWWH013-04 Tankless Water Heater_DMo_Ex/renamed_cohort.xlsx
+++ b/residential measures/SWWH013-04 Tankless Water Heater/SWWH013-04 Tankless Water Heater_DMo_Ex/renamed_cohort.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEER-SWWH012-03\residential measures\SWWH012-03 Storage Water Heater\SWWH012-03 Storage Water Heater_SFm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEER-SWWH013\residential measures\SWWH013-04 Tankless Water Heater\SWWH013-04 Tankless Water Heater_DMo_Ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A7CB51-DA0F-455D-8F6A-09DD307A688A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75631C81-6C45-4799-875D-471CB0D8809E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>WaterHtg_eq</t>
   </si>
   <si>
-    <t>Stor_UEF</t>
+    <t>Instant_UEF</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="G2" t="str">
         <f>A2&amp;"&amp;"&amp;B2&amp;"&amp;"&amp;C2&amp;"&amp;"&amp;D2&amp;"&amp;"&amp;E2&amp;"__"&amp;F2</f>
-        <v>SFm&amp;1&amp;DXGF&amp;Ex&amp;WaterHtg_eq__Stor_UEF</v>
+        <v>SFm&amp;1&amp;DXGF&amp;Ex&amp;WaterHtg_eq__Instant_UEF</v>
       </c>
     </row>
   </sheetData>

</xml_diff>